<commit_message>
forsøg på at lave grafer til FCT, det gik galt med conc magic
</commit_message>
<xml_diff>
--- a/data/FCT/start_concentration.xlsx
+++ b/data/FCT/start_concentration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grundfos-my.sharepoint.com/personal/102222_grundfos_com/Documents/Desktop/Speciale/data/FCT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{6287A363-5042-46E7-AAC9-2D66BA34D331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC80B96A-50D5-452C-8194-9D193F296B21}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{6287A363-5042-46E7-AAC9-2D66BA34D331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34DBE23E-B087-44D5-B1AC-364DE633D995}"/>
   <bookViews>
-    <workbookView xWindow="3435" yWindow="2085" windowWidth="21600" windowHeight="11385" xr2:uid="{2CD68D51-4BE6-497F-8779-5747913E4722}"/>
+    <workbookView xWindow="-22650" yWindow="1155" windowWidth="21600" windowHeight="11385" xr2:uid="{2CD68D51-4BE6-497F-8779-5747913E4722}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -434,7 +434,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>